<commit_message>
Archivos que no había subido.
</commit_message>
<xml_diff>
--- a/ges/Estimaciones por historias.xlsx
+++ b/ges/Estimaciones por historias.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Estimaciones</t>
   </si>
@@ -52,13 +52,19 @@
   </si>
   <si>
     <t>Tema</t>
+  </si>
+  <si>
+    <t>Buffer</t>
+  </si>
+  <si>
+    <t>Total con buffer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +72,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -83,15 +115,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -390,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -402,63 +547,143 @@
     <col min="2" max="2" width="26.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1.1499999999999999</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3">
+      <c r="C3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
         <f>(C3+(4*D3)+E3)/6</f>
-        <v>0</v>
+        <v>1.25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" ref="F4:F6" si="0">(C4+(4*D4)+E4)/6</f>
+        <v>3.3333333333333335</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <f>SUM(F3:F6)*I2</f>
+        <v>10.0625</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>